<commit_message>
0403 Class are fully functional for sensitivity analyses
</commit_message>
<xml_diff>
--- a/A_low.xlsx
+++ b/A_low.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,25 +467,30 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Journey Time Benefit</t>
+          <t>Journey Time Work Benefit</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Journey Time Non Work Benefit</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Emission Benefit</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>All Benefit</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Maintenance Cost</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Construction Cost</t>
         </is>
@@ -496,33 +501,36 @@
         <v>2031</v>
       </c>
       <c r="B2" t="n">
-        <v>-41194.58184790942</v>
+        <v>-25921.19411456322</v>
       </c>
       <c r="C2" t="n">
-        <v>7877.945861321523</v>
+        <v>4957.102481322999</v>
       </c>
       <c r="D2" t="n">
-        <v>-736061.6794333999</v>
+        <v>-772864.7634050698</v>
       </c>
       <c r="E2" t="n">
-        <v>491335.2625454253</v>
+        <v>-491335.2625454253</v>
       </c>
       <c r="F2" t="n">
-        <v>4907.077862889333</v>
+        <v>-5152.4317560338</v>
       </c>
       <c r="G2" t="n">
-        <v>9711888.62031826</v>
+        <v>323887.7094811517</v>
       </c>
       <c r="H2" t="n">
-        <v>145079.5284625217</v>
+        <v>6695668.300280038</v>
       </c>
       <c r="I2" t="n">
-        <v>9574018.01804333</v>
+        <v>-145079.5284625217</v>
       </c>
       <c r="J2" t="n">
-        <v>15893</v>
+        <v>5584159.931958899</v>
       </c>
       <c r="K2" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L2" t="n">
         <v>145540147.5</v>
       </c>
     </row>
@@ -531,1947 +539,2124 @@
         <v>2032</v>
       </c>
       <c r="B3" t="n">
-        <v>-41431.6580086062</v>
+        <v>-26070.37143123183</v>
       </c>
       <c r="C3" t="n">
-        <v>7956.725319934739</v>
+        <v>5006.67350613623</v>
       </c>
       <c r="D3" t="n">
-        <v>-740297.73838019</v>
+        <v>-777312.6252991996</v>
       </c>
       <c r="E3" t="n">
-        <v>496248.6151708795</v>
+        <v>-496248.6151708795</v>
       </c>
       <c r="F3" t="n">
-        <v>4935.318255867934</v>
+        <v>-5182.084168661331</v>
       </c>
       <c r="G3" t="n">
-        <v>9956142.619119257</v>
+        <v>332033.4853746028</v>
       </c>
       <c r="H3" t="n">
-        <v>122796.3609287939</v>
+        <v>6864064.35803208</v>
       </c>
       <c r="I3" t="n">
-        <v>9796479.605894201</v>
+        <v>-122796.3609287939</v>
       </c>
       <c r="J3" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K3" t="inlineStr"/>
+        <v>5773494.459914053</v>
+      </c>
+      <c r="K3" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>2033</v>
       </c>
       <c r="B4" t="n">
-        <v>-42025.32180575933</v>
+        <v>-26443.92722023363</v>
       </c>
       <c r="C4" t="n">
-        <v>8036.292573134087</v>
+        <v>5056.740241197592</v>
       </c>
       <c r="D4" t="n">
-        <v>-750905.2783029076</v>
+        <v>-788450.5422180528</v>
       </c>
       <c r="E4" t="n">
-        <v>501211.1013225882</v>
+        <v>-501211.1013225882</v>
       </c>
       <c r="F4" t="n">
-        <v>5006.035188686052</v>
+        <v>-5256.336948120353</v>
       </c>
       <c r="G4" t="n">
-        <v>10206539.60599011</v>
+        <v>340384.1275317738</v>
       </c>
       <c r="H4" t="n">
-        <v>104006.4255996393</v>
+        <v>7036695.576636588</v>
       </c>
       <c r="I4" t="n">
-        <v>10021856.79018812</v>
+        <v>-104006.4255996393</v>
       </c>
       <c r="J4" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K4" t="inlineStr"/>
+        <v>5956768.111100925</v>
+      </c>
+      <c r="K4" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>2034</v>
       </c>
       <c r="B5" t="n">
-        <v>-42849.38479832956</v>
+        <v>-26962.45892597844</v>
       </c>
       <c r="C5" t="n">
-        <v>8116.655498865392</v>
+        <v>5107.307643609544</v>
       </c>
       <c r="D5" t="n">
-        <v>-765629.5736607191</v>
+        <v>-803911.052343755</v>
       </c>
       <c r="E5" t="n">
-        <v>506223.2123358143</v>
+        <v>-506223.2123358143</v>
       </c>
       <c r="F5" t="n">
-        <v>5104.197157738128</v>
+        <v>-5359.407015625035</v>
       </c>
       <c r="G5" t="n">
-        <v>10463234.07708076</v>
+        <v>348944.7883391981</v>
       </c>
       <c r="H5" t="n">
-        <v>88128.75284915058</v>
+        <v>7213668.470389002</v>
       </c>
       <c r="I5" t="n">
-        <v>10252119.54214781</v>
+        <v>-88128.75284915058</v>
       </c>
       <c r="J5" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K5" t="inlineStr"/>
+        <v>6137135.682901487</v>
+      </c>
+      <c r="K5" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>2035</v>
       </c>
       <c r="B6" t="n">
-        <v>-42558.94834717164</v>
+        <v>-26779.70528968219</v>
       </c>
       <c r="C6" t="n">
-        <v>8197.822053854083</v>
+        <v>5158.380720045664</v>
       </c>
       <c r="D6" t="n">
-        <v>-760440.0770711612</v>
+        <v>-798462.0809247198</v>
       </c>
       <c r="E6" t="n">
-        <v>511285.4444591723</v>
+        <v>-511285.4444591723</v>
       </c>
       <c r="F6" t="n">
-        <v>5069.600513807742</v>
+        <v>-5323.080539498133</v>
       </c>
       <c r="G6" t="n">
-        <v>10726384.41411934</v>
+        <v>357720.7497659288</v>
       </c>
       <c r="H6" t="n">
-        <v>74694.93689665546</v>
+        <v>7395092.232419278</v>
       </c>
       <c r="I6" t="n">
-        <v>10512493.99159688</v>
+        <v>-74694.93689665546</v>
       </c>
       <c r="J6" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K6" t="inlineStr"/>
+        <v>6341426.114795525</v>
+      </c>
+      <c r="K6" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>2036</v>
       </c>
       <c r="B7" t="n">
-        <v>-42562.80908152481</v>
+        <v>-26782.13461024096</v>
       </c>
       <c r="C7" t="n">
-        <v>8279.800274392623</v>
+        <v>5209.964527246119</v>
       </c>
       <c r="D7" t="n">
-        <v>-760509.0603812073</v>
+        <v>-798534.5134002677</v>
       </c>
       <c r="E7" t="n">
-        <v>516398.2989037641</v>
+        <v>-516398.2989037641</v>
       </c>
       <c r="F7" t="n">
-        <v>5070.060402541382</v>
+        <v>-5323.563422668452</v>
       </c>
       <c r="G7" t="n">
-        <v>10996152.98213444</v>
+        <v>366717.4266225419</v>
       </c>
       <c r="H7" t="n">
-        <v>63315.26136170374</v>
+        <v>7581078.802064621</v>
       </c>
       <c r="I7" t="n">
-        <v>10776004.41280902</v>
+        <v>-63315.26136170374</v>
       </c>
       <c r="J7" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K7" t="inlineStr"/>
+        <v>6542652.421515765</v>
+      </c>
+      <c r="K7" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>2037</v>
       </c>
       <c r="B8" t="n">
-        <v>-41557.77900614378</v>
+        <v>-26149.73154881147</v>
       </c>
       <c r="C8" t="n">
-        <v>8362.598277136551</v>
+        <v>5262.064172518582</v>
       </c>
       <c r="D8" t="n">
-        <v>-742551.2588456259</v>
+        <v>-779678.821787907</v>
       </c>
       <c r="E8" t="n">
-        <v>521562.2818928018</v>
+        <v>-521562.2818928018</v>
       </c>
       <c r="F8" t="n">
-        <v>4950.341725637507</v>
+        <v>-5197.858811919381</v>
       </c>
       <c r="G8" t="n">
-        <v>11272706.22963513</v>
+        <v>375940.369902099</v>
       </c>
       <c r="H8" t="n">
-        <v>53666.16141625639</v>
+        <v>7771742.933936553</v>
       </c>
       <c r="I8" t="n">
-        <v>11067237.89164391</v>
+        <v>-53666.16141625639</v>
       </c>
       <c r="J8" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K8" t="inlineStr"/>
+        <v>6766690.512553474</v>
+      </c>
+      <c r="K8" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>2038</v>
       </c>
       <c r="B9" t="n">
-        <v>-42152.94920700453</v>
+        <v>-26524.23522418979</v>
       </c>
       <c r="C9" t="n">
-        <v>8446.224259907916</v>
+        <v>5314.684814243767</v>
       </c>
       <c r="D9" t="n">
-        <v>-753185.7150760997</v>
+        <v>-790845.0008299048</v>
       </c>
       <c r="E9" t="n">
-        <v>526777.9047117297</v>
+        <v>-526777.9047117297</v>
       </c>
       <c r="F9" t="n">
-        <v>5021.238100507331</v>
+        <v>-5272.300005532699</v>
       </c>
       <c r="G9" t="n">
-        <v>11556214.79131045</v>
+        <v>385395.2702051366</v>
       </c>
       <c r="H9" t="n">
-        <v>45487.82725854934</v>
+        <v>7967202.268725057</v>
       </c>
       <c r="I9" t="n">
-        <v>11336566.84515702</v>
+        <v>-45487.82725854934</v>
       </c>
       <c r="J9" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K9" t="inlineStr"/>
+        <v>6963004.955714531</v>
+      </c>
+      <c r="K9" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>2039</v>
       </c>
       <c r="B10" t="n">
-        <v>-41922.9675204101</v>
+        <v>-26379.52201984126</v>
       </c>
       <c r="C10" t="n">
-        <v>8530.686502506993</v>
+        <v>5367.831662386205</v>
       </c>
       <c r="D10" t="n">
-        <v>-749076.419657139</v>
+        <v>-786530.2406399964</v>
       </c>
       <c r="E10" t="n">
-        <v>532045.6837588472</v>
+        <v>-532045.6837588472</v>
       </c>
       <c r="F10" t="n">
-        <v>4993.842797714261</v>
+        <v>-5243.534937599977</v>
       </c>
       <c r="G10" t="n">
-        <v>11846853.5933119</v>
+        <v>395087.9612507956</v>
       </c>
       <c r="H10" t="n">
-        <v>38557.23095533584</v>
+        <v>8167577.405783485</v>
       </c>
       <c r="I10" t="n">
-        <v>11629993.96455333</v>
+        <v>-38557.23095533584</v>
       </c>
       <c r="J10" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K10" t="inlineStr"/>
+        <v>7179276.986385046</v>
+      </c>
+      <c r="K10" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>2040</v>
       </c>
       <c r="B11" t="n">
-        <v>-43144.92578971171</v>
+        <v>-27148.4245326864</v>
       </c>
       <c r="C11" t="n">
-        <v>8615.993367532026</v>
+        <v>5421.509979010042</v>
       </c>
       <c r="D11" t="n">
-        <v>-770910.2777897546</v>
+        <v>-809455.7916792425</v>
       </c>
       <c r="E11" t="n">
-        <v>537366.1405964353</v>
+        <v>-537366.1405964353</v>
       </c>
       <c r="F11" t="n">
-        <v>5139.401851931698</v>
+        <v>-5396.371944528284</v>
       </c>
       <c r="G11" t="n">
-        <v>12144801.9611837</v>
+        <v>405024.4234762533</v>
       </c>
       <c r="H11" t="n">
-        <v>32680.21016139772</v>
+        <v>8372991.977538947</v>
       </c>
       <c r="I11" t="n">
-        <v>11904269.69987766</v>
+        <v>-32680.21016139772</v>
       </c>
       <c r="J11" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K11" t="inlineStr"/>
+        <v>7371390.97207992</v>
+      </c>
+      <c r="K11" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>2041</v>
       </c>
       <c r="B12" t="n">
-        <v>-42619.94095528748</v>
+        <v>-26818.08415320267</v>
       </c>
       <c r="C12" t="n">
-        <v>8702.153301207345</v>
+        <v>5475.725078800143</v>
       </c>
       <c r="D12" t="n">
-        <v>-761529.88838976</v>
+        <v>-799606.3828092478</v>
       </c>
       <c r="E12" t="n">
-        <v>542739.8020023998</v>
+        <v>-542739.8020023998</v>
       </c>
       <c r="F12" t="n">
-        <v>5076.8659225984</v>
+        <v>-5330.70921872832</v>
       </c>
       <c r="G12" t="n">
-        <v>12450243.73050746</v>
+        <v>415210.7877266811</v>
       </c>
       <c r="H12" t="n">
-        <v>31713.06156806759</v>
+        <v>8583572.725774044</v>
       </c>
       <c r="I12" t="n">
-        <v>12224172.05211149</v>
+        <v>-31713.06156806759</v>
       </c>
       <c r="J12" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K12" t="inlineStr"/>
+        <v>7598051.19882788</v>
+      </c>
+      <c r="K12" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>2042</v>
       </c>
       <c r="B13" t="n">
-        <v>-42751.05329672187</v>
+        <v>-26900.58501376931</v>
       </c>
       <c r="C13" t="n">
-        <v>8789.174834219497</v>
+        <v>5530.482329588193</v>
       </c>
       <c r="D13" t="n">
-        <v>-763872.5938112375</v>
+        <v>-802066.2235017995</v>
       </c>
       <c r="E13" t="n">
-        <v>548167.2000224238</v>
+        <v>-548167.2000224238</v>
       </c>
       <c r="F13" t="n">
-        <v>5092.483958741583</v>
+        <v>-5347.108156678664</v>
       </c>
       <c r="G13" t="n">
-        <v>12763367.36032972</v>
+        <v>425653.3390380071</v>
       </c>
       <c r="H13" t="n">
-        <v>30653.83559936468</v>
+        <v>8799449.579827266</v>
       </c>
       <c r="I13" t="n">
-        <v>12539261.43971903</v>
+        <v>-30653.83559936468</v>
       </c>
       <c r="J13" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K13" t="inlineStr"/>
+        <v>7817498.448900825</v>
+      </c>
+      <c r="K13" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>2043</v>
       </c>
       <c r="B14" t="n">
-        <v>-42799.90395519092</v>
+        <v>-26931.32370181998</v>
       </c>
       <c r="C14" t="n">
-        <v>8877.066582561651</v>
+        <v>5585.787152884051</v>
       </c>
       <c r="D14" t="n">
-        <v>-764745.4536899204</v>
+        <v>-802982.7263744166</v>
       </c>
       <c r="E14" t="n">
-        <v>553648.8720226479</v>
+        <v>-553648.8720226479</v>
       </c>
       <c r="F14" t="n">
-        <v>5098.30302459947</v>
+        <v>-5353.218175829445</v>
       </c>
       <c r="G14" t="n">
-        <v>13084366.04944202</v>
+        <v>436358.5205148127</v>
       </c>
       <c r="H14" t="n">
-        <v>19644.77970941094</v>
+        <v>9020755.736759922</v>
       </c>
       <c r="I14" t="n">
-        <v>12853893.10708693</v>
+        <v>-19644.77970941094</v>
       </c>
       <c r="J14" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K14" t="inlineStr"/>
+        <v>8054139.124443494</v>
+      </c>
+      <c r="K14" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>2044</v>
       </c>
       <c r="B15" t="n">
-        <v>-43397.68031755753</v>
+        <v>-27307.46727291411</v>
       </c>
       <c r="C15" t="n">
-        <v>8965.83724838727</v>
+        <v>5641.645024412891</v>
       </c>
       <c r="D15" t="n">
-        <v>-775426.4766174897</v>
+        <v>-814197.8004483643</v>
       </c>
       <c r="E15" t="n">
-        <v>559185.3607428746</v>
+        <v>-559185.3607428746</v>
       </c>
       <c r="F15" t="n">
-        <v>5169.509844116598</v>
+        <v>-5427.98533632243</v>
       </c>
       <c r="G15" t="n">
-        <v>13413437.85558548</v>
+        <v>447332.9373057602</v>
       </c>
       <c r="H15" t="n">
-        <v>18598.17001726007</v>
+        <v>9247627.743539426</v>
       </c>
       <c r="I15" t="n">
-        <v>13176193.55681483</v>
+        <v>-18598.17001726007</v>
       </c>
       <c r="J15" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K15" t="inlineStr"/>
+        <v>8275885.542051864</v>
+      </c>
+      <c r="K15" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>2045</v>
       </c>
       <c r="B16" t="n">
-        <v>-42610.53507016502</v>
+        <v>-26812.16561335733</v>
       </c>
       <c r="C16" t="n">
-        <v>9055.495620871105</v>
+        <v>5698.061474656996</v>
       </c>
       <c r="D16" t="n">
-        <v>-761361.8247442684</v>
+        <v>-799429.915981482</v>
       </c>
       <c r="E16" t="n">
-        <v>564777.2143503034</v>
+        <v>-564777.2143503034</v>
       </c>
       <c r="F16" t="n">
-        <v>5075.745498295124</v>
+        <v>-5329.53277320988</v>
       </c>
       <c r="G16" t="n">
-        <v>13750785.81765346</v>
+        <v>458583.3606790002</v>
       </c>
       <c r="H16" t="n">
-        <v>17614.10384290229</v>
+        <v>9480205.581289442</v>
       </c>
       <c r="I16" t="n">
-        <v>13533184.5261548</v>
+        <v>-17614.10384290229</v>
       </c>
       <c r="J16" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K16" t="inlineStr"/>
+        <v>8530524.070881844</v>
+      </c>
+      <c r="K16" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>2046</v>
       </c>
       <c r="B17" t="n">
-        <v>-43575.27305711117</v>
+        <v>-27419.21536377478</v>
       </c>
       <c r="C17" t="n">
-        <v>9146.050577079854</v>
+        <v>5755.042089403591</v>
       </c>
       <c r="D17" t="n">
-        <v>-778599.6902846083</v>
+        <v>-817529.6747988388</v>
       </c>
       <c r="E17" t="n">
-        <v>570424.9864938064</v>
+        <v>-570424.9864938064</v>
       </c>
       <c r="F17" t="n">
-        <v>5190.66460189739</v>
+        <v>-5450.197831992259</v>
       </c>
       <c r="G17" t="n">
-        <v>14096618.08096743</v>
+        <v>470116.7322000769</v>
       </c>
       <c r="H17" t="n">
-        <v>17551.47794671069</v>
+        <v>9718632.751658874</v>
       </c>
       <c r="I17" t="n">
-        <v>13866374.96804141</v>
+        <v>-17551.47794671069</v>
       </c>
       <c r="J17" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K17" t="inlineStr"/>
+        <v>8756128.973513233</v>
+      </c>
+      <c r="K17" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>2047</v>
       </c>
       <c r="B18" t="n">
-        <v>-43054.5218281202</v>
+        <v>-27091.53892948279</v>
       </c>
       <c r="C18" t="n">
-        <v>9237.511082850651</v>
+        <v>5812.592510297627</v>
       </c>
       <c r="D18" t="n">
-        <v>-769294.9466269779</v>
+        <v>-807759.6939583271</v>
       </c>
       <c r="E18" t="n">
-        <v>576129.2363587447</v>
+        <v>-576129.2363587447</v>
       </c>
       <c r="F18" t="n">
-        <v>5128.632977513186</v>
+        <v>-5385.064626388848</v>
       </c>
       <c r="G18" t="n">
-        <v>14451148.02570377</v>
+        <v>481940.1680149089</v>
       </c>
       <c r="H18" t="n">
-        <v>12361.542297729</v>
+        <v>9963056.365363086</v>
       </c>
       <c r="I18" t="n">
-        <v>14231398.21401048</v>
+        <v>-12361.542297729</v>
       </c>
       <c r="J18" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K18" t="inlineStr"/>
+        <v>9022082.04971762</v>
+      </c>
+      <c r="K18" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>2048</v>
       </c>
       <c r="B19" t="n">
-        <v>-42152.52562976319</v>
+        <v>-26523.968693316</v>
       </c>
       <c r="C19" t="n">
-        <v>9329.886193679158</v>
+        <v>5870.718435400601</v>
       </c>
       <c r="D19" t="n">
-        <v>-753178.1466299198</v>
+        <v>-790837.0539614153</v>
       </c>
       <c r="E19" t="n">
-        <v>581890.528722332</v>
+        <v>-581890.528722332</v>
       </c>
       <c r="F19" t="n">
-        <v>5021.187644199465</v>
+        <v>-5272.247026409436</v>
       </c>
       <c r="G19" t="n">
-        <v>14814594.39855022</v>
+        <v>494060.9632404837</v>
       </c>
       <c r="H19" t="n">
-        <v>12248.55172720564</v>
+        <v>10213627.23295197</v>
       </c>
       <c r="I19" t="n">
-        <v>14617711.50528955</v>
+        <v>-12248.55172720564</v>
       </c>
       <c r="J19" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K19" t="inlineStr"/>
+        <v>9296786.564497178</v>
+      </c>
+      <c r="K19" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>2049</v>
       </c>
       <c r="B20" t="n">
-        <v>-43091.38654694115</v>
+        <v>-27114.73560947495</v>
       </c>
       <c r="C20" t="n">
-        <v>9423.18505561595</v>
+        <v>5929.425619754609</v>
       </c>
       <c r="D20" t="n">
-        <v>-769953.6426406282</v>
+        <v>-808451.3247726593</v>
       </c>
       <c r="E20" t="n">
-        <v>587709.4340095553</v>
+        <v>-587709.4340095553</v>
       </c>
       <c r="F20" t="n">
-        <v>5133.024284270855</v>
+        <v>-5389.675498484396</v>
       </c>
       <c r="G20" t="n">
-        <v>15187181.44767376</v>
+        <v>506486.5964659819</v>
       </c>
       <c r="H20" t="n">
-        <v>7916.616275117605</v>
+        <v>10470499.95786072</v>
       </c>
       <c r="I20" t="n">
-        <v>14974052.62954221</v>
+        <v>-7916.616275117605</v>
       </c>
       <c r="J20" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K20" t="inlineStr"/>
+        <v>9546334.193781162</v>
+      </c>
+      <c r="K20" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>2050</v>
       </c>
       <c r="B21" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C21" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D21" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E21" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F21" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G21" t="n">
-        <v>15569139.06108274</v>
+        <v>519224.7343671013</v>
       </c>
       <c r="H21" t="n">
-        <v>6145.496508111467</v>
+        <v>10733833.03180092</v>
       </c>
       <c r="I21" t="n">
-        <v>15372401.92056438</v>
+        <v>-6145.496508111467</v>
       </c>
       <c r="J21" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K21" t="inlineStr"/>
+        <v>9830889.601173211</v>
+      </c>
+      <c r="K21" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
         <v>2051</v>
       </c>
       <c r="B22" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C22" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D22" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E22" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F22" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G22" t="n">
-        <v>15802676.14699899</v>
+        <v>527013.1053826079</v>
       </c>
       <c r="H22" t="n">
-        <v>6237.678954729924</v>
+        <v>10894840.52727793</v>
       </c>
       <c r="I22" t="n">
-        <v>15606031.18892724</v>
+        <v>-6237.678954729924</v>
       </c>
       <c r="J22" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K22" t="inlineStr"/>
+        <v>9999593.285219116</v>
+      </c>
+      <c r="K22" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
         <v>2052</v>
       </c>
       <c r="B23" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C23" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D23" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E23" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F23" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G23" t="n">
-        <v>16039716.28920397</v>
+        <v>534918.3019633468</v>
       </c>
       <c r="H23" t="n">
-        <v>6331.244139809604</v>
+        <v>11058263.1351871</v>
       </c>
       <c r="I23" t="n">
-        <v>15843164.8963173</v>
+        <v>-6331.244139809604</v>
       </c>
       <c r="J23" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K23" t="inlineStr"/>
+        <v>10170827.52452394</v>
+      </c>
+      <c r="K23" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
         <v>2053</v>
       </c>
       <c r="B24" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C24" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D24" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E24" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F24" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G24" t="n">
-        <v>16280312.03354203</v>
+        <v>542942.0764927971</v>
       </c>
       <c r="H24" t="n">
-        <v>6426.212802075356</v>
+        <v>11224137.0822149</v>
       </c>
       <c r="I24" t="n">
-        <v>16083855.60931763</v>
+        <v>-6426.212802075356</v>
       </c>
       <c r="J24" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K24" t="inlineStr"/>
+        <v>10344630.27741893</v>
+      </c>
+      <c r="K24" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
         <v>2054</v>
       </c>
       <c r="B25" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C25" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D25" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E25" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F25" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G25" t="n">
-        <v>16524516.71404515</v>
+        <v>551086.207640189</v>
       </c>
       <c r="H25" t="n">
-        <v>6522.605993862005</v>
+        <v>11392499.13844812</v>
       </c>
       <c r="I25" t="n">
-        <v>16328156.68301254</v>
+        <v>-6522.605993862005</v>
       </c>
       <c r="J25" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K25" t="inlineStr"/>
+        <v>10521040.07160776</v>
+      </c>
+      <c r="K25" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
         <v>2055</v>
       </c>
       <c r="B26" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C26" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D26" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E26" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F26" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G26" t="n">
-        <v>16772384.46475583</v>
+        <v>559352.5007547918</v>
       </c>
       <c r="H26" t="n">
-        <v>6620.445082800444</v>
+        <v>11563386.62552484</v>
       </c>
       <c r="I26" t="n">
-        <v>16576122.27281215</v>
+        <v>-6620.445082800444</v>
       </c>
       <c r="J26" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K26" t="inlineStr"/>
+        <v>10700096.01271014</v>
+      </c>
+      <c r="K26" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
         <v>2056</v>
       </c>
       <c r="B27" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C27" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D27" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E27" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F27" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G27" t="n">
-        <v>17023970.23172716</v>
+        <v>567742.7882661133</v>
       </c>
       <c r="H27" t="n">
-        <v>6719.751760247992</v>
+        <v>11736837.42490771</v>
       </c>
       <c r="I27" t="n">
-        <v>16827807.34646094</v>
+        <v>-6719.751760247992</v>
       </c>
       <c r="J27" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K27" t="inlineStr"/>
+        <v>10881837.79292688</v>
+      </c>
+      <c r="K27" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
         <v>2057</v>
       </c>
       <c r="B28" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C28" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D28" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E28" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F28" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G28" t="n">
-        <v>17279329.78520307</v>
+        <v>576258.9300901048</v>
       </c>
       <c r="H28" t="n">
-        <v>6820.548036230193</v>
+        <v>11912889.98628133</v>
       </c>
       <c r="I28" t="n">
-        <v>17083267.69621283</v>
+        <v>-6820.548036230193</v>
       </c>
       <c r="J28" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K28" t="inlineStr"/>
+        <v>11066305.69984851</v>
+      </c>
+      <c r="K28" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
         <v>2058</v>
       </c>
       <c r="B29" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C29" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D29" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E29" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F29" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G29" t="n">
-        <v>17538519.73198112</v>
+        <v>584902.8140414567</v>
       </c>
       <c r="H29" t="n">
-        <v>6922.856256301546</v>
+        <v>12091583.33607555</v>
       </c>
       <c r="I29" t="n">
-        <v>17342559.95121095</v>
+        <v>-6922.856256301546</v>
       </c>
       <c r="J29" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K29" t="inlineStr"/>
+        <v>11253540.62537401</v>
+      </c>
+      <c r="K29" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
         <v>2059</v>
       </c>
       <c r="B30" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C30" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D30" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E30" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F30" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G30" t="n">
-        <v>17801597.52796084</v>
+        <v>593676.3562520782</v>
       </c>
       <c r="H30" t="n">
-        <v>7026.699099859435</v>
+        <v>12272957.08611668</v>
       </c>
       <c r="I30" t="n">
-        <v>17605741.59003422</v>
+        <v>-7026.699099859435</v>
       </c>
       <c r="J30" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K30" t="inlineStr"/>
+        <v>11443584.07478221</v>
+      </c>
+      <c r="K30" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
         <v>2060</v>
       </c>
       <c r="B31" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C31" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D31" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E31" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F31" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G31" t="n">
-        <v>18068621.49088024</v>
+        <v>602581.5015958595</v>
       </c>
       <c r="H31" t="n">
-        <v>7132.099586888442</v>
+        <v>12457051.44240843</v>
       </c>
       <c r="I31" t="n">
-        <v>17872870.95344066</v>
+        <v>-7132.099586888442</v>
       </c>
       <c r="J31" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K31" t="inlineStr"/>
+        <v>11636478.17593071</v>
+      </c>
+      <c r="K31" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
         <v>2061</v>
       </c>
       <c r="B32" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C32" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D32" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E32" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F32" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G32" t="n">
-        <v>18339650.81324345</v>
+        <v>611620.2241197971</v>
       </c>
       <c r="H32" t="n">
-        <v>7239.081081332477</v>
+        <v>12643907.21404455</v>
       </c>
       <c r="I32" t="n">
-        <v>18144007.25729831</v>
+        <v>-7239.081081332477</v>
       </c>
       <c r="J32" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K32" t="inlineStr"/>
+        <v>11832265.68859632</v>
+      </c>
+      <c r="K32" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
         <v>2062</v>
       </c>
       <c r="B33" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C33" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D33" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E33" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F33" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G33" t="n">
-        <v>18614745.5754421</v>
+        <v>620794.5274815942</v>
       </c>
       <c r="H33" t="n">
-        <v>7347.667296153025</v>
+        <v>12833565.82225522</v>
       </c>
       <c r="I33" t="n">
-        <v>18419210.60571178</v>
+        <v>-7347.667296153025</v>
       </c>
       <c r="J33" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K33" t="inlineStr"/>
+        <v>12030990.01395397</v>
+      </c>
+      <c r="K33" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
         <v>2063</v>
       </c>
       <c r="B34" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C34" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D34" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E34" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F34" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G34" t="n">
-        <v>18893966.75907372</v>
+        <v>630106.4453938182</v>
       </c>
       <c r="H34" t="n">
-        <v>7457.88230681772</v>
+        <v>13026069.30958905</v>
       </c>
       <c r="I34" t="n">
-        <v>18698542.00435407</v>
+        <v>-7457.88230681772</v>
       </c>
       <c r="J34" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K34" t="inlineStr"/>
+        <v>12232695.20418935</v>
+      </c>
+      <c r="K34" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
         <v>2064</v>
       </c>
       <c r="B35" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C35" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D35" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E35" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F35" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G35" t="n">
-        <v>19177376.26045983</v>
+        <v>639558.0420747256</v>
       </c>
       <c r="H35" t="n">
-        <v>7569.750541183937</v>
+        <v>13221460.34923289</v>
       </c>
       <c r="I35" t="n">
-        <v>18982063.37397454</v>
+        <v>-7569.750541183937</v>
       </c>
       <c r="J35" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K35" t="inlineStr"/>
+        <v>12437425.97227974</v>
+      </c>
+      <c r="K35" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
         <v>2065</v>
       </c>
       <c r="B36" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C36" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D36" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E36" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F36" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G36" t="n">
-        <v>19465036.90436672</v>
+        <v>649151.412705846</v>
       </c>
       <c r="H36" t="n">
-        <v>7683.296799731645</v>
+        <v>13419782.25447137</v>
       </c>
       <c r="I36" t="n">
-        <v>19269837.56413998</v>
+        <v>-7683.296799731645</v>
       </c>
       <c r="J36" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K36" t="inlineStr"/>
+        <v>12645227.70189079</v>
+      </c>
+      <c r="K36" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
         <v>2066</v>
       </c>
       <c r="B37" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C37" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D37" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E37" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F37" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G37" t="n">
-        <v>19757012.45793223</v>
+        <v>658888.6838964339</v>
       </c>
       <c r="H37" t="n">
-        <v>7798.546250505218</v>
+        <v>13621078.98828845</v>
       </c>
       <c r="I37" t="n">
-        <v>19561928.36715626</v>
+        <v>-7798.546250505218</v>
       </c>
       <c r="J37" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K37" t="inlineStr"/>
+        <v>12856146.45744768</v>
+      </c>
+      <c r="K37" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
         <v>2067</v>
       </c>
       <c r="B38" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C38" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D38" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E38" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F38" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G38" t="n">
-        <v>20053367.6448012</v>
+        <v>668772.0141548804</v>
       </c>
       <c r="H38" t="n">
-        <v>7915.524444288087</v>
+        <v>13825395.17311278</v>
       </c>
       <c r="I38" t="n">
-        <v>19858400.53221902</v>
+        <v>-7915.524444288087</v>
       </c>
       <c r="J38" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K38" t="inlineStr"/>
+        <v>13070228.99433667</v>
+      </c>
+      <c r="K38" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
         <v>2068</v>
       </c>
       <c r="B39" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C39" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D39" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E39" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F39" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G39" t="n">
-        <v>20354168.15947321</v>
+        <v>678803.5943672037</v>
       </c>
       <c r="H39" t="n">
-        <v>8034.257311230614</v>
+        <v>14032776.10070947</v>
       </c>
       <c r="I39" t="n">
-        <v>20159319.77975797</v>
+        <v>-8034.257311230614</v>
       </c>
       <c r="J39" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K39" t="inlineStr"/>
+        <v>13287522.76927875</v>
+      </c>
+      <c r="K39" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
         <v>2069</v>
       </c>
       <c r="B40" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C40" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D40" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E40" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F40" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G40" t="n">
-        <v>20659480.68186532</v>
+        <v>688985.6482827119</v>
       </c>
       <c r="H40" t="n">
-        <v>8154.771170966511</v>
+        <v>14243267.74222011</v>
       </c>
       <c r="I40" t="n">
-        <v>20464752.81600982</v>
+        <v>-8154.771170966511</v>
       </c>
       <c r="J40" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K40" t="inlineStr"/>
+        <v>13508075.95084516</v>
+      </c>
+      <c r="K40" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
         <v>2070</v>
       </c>
       <c r="B41" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C41" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D41" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E41" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F41" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G41" t="n">
-        <v>20969372.8920933</v>
+        <v>699320.4330069518</v>
       </c>
       <c r="H41" t="n">
-        <v>8277.092739357184</v>
+        <v>14456916.75835339</v>
       </c>
       <c r="I41" t="n">
-        <v>20774767.34780618</v>
+        <v>-8277.092739357184</v>
       </c>
       <c r="J41" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K41" t="inlineStr"/>
+        <v>13731937.43013429</v>
+      </c>
+      <c r="K41" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
         <v>2071</v>
       </c>
       <c r="B42" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C42" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D42" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E42" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F42" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G42" t="n">
-        <v>21283913.4854747</v>
+        <v>709810.2395020563</v>
       </c>
       <c r="H42" t="n">
-        <v>8401.249130177772</v>
+        <v>14673770.5097287</v>
       </c>
       <c r="I42" t="n">
-        <v>21089432.0975784</v>
+        <v>-8401.249130177772</v>
       </c>
       <c r="J42" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K42" t="inlineStr"/>
+        <v>13959156.83161388</v>
+      </c>
+      <c r="K42" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
         <v>2072</v>
       </c>
       <c r="B43" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C43" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D43" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E43" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F43" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G43" t="n">
-        <v>21603172.18775682</v>
+        <v>720457.3930945871</v>
       </c>
       <c r="H43" t="n">
-        <v>8527.267866919678</v>
+        <v>14893877.06737462</v>
       </c>
       <c r="I43" t="n">
-        <v>21408816.81859726</v>
+        <v>-8527.267866919678</v>
       </c>
       <c r="J43" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K43" t="inlineStr"/>
+        <v>14189784.5241156</v>
+      </c>
+      <c r="K43" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
         <v>2073</v>
       </c>
       <c r="B44" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C44" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D44" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E44" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F44" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G44" t="n">
-        <v>21927219.77057317</v>
+        <v>731264.2539910054</v>
       </c>
       <c r="H44" t="n">
-        <v>8655.176884476665</v>
+        <v>15117285.22338525</v>
       </c>
       <c r="I44" t="n">
-        <v>21732992.31043117</v>
+        <v>-8655.176884476665</v>
       </c>
       <c r="J44" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K44" t="inlineStr"/>
+        <v>14423871.63200508</v>
+      </c>
+      <c r="K44" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
         <v>2074</v>
       </c>
       <c r="B45" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C45" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D45" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E45" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F45" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G45" t="n">
-        <v>22256128.06713176</v>
+        <v>742233.2178008707</v>
       </c>
       <c r="H45" t="n">
-        <v>8785.004537575207</v>
+        <v>15344044.50173603</v>
       </c>
       <c r="I45" t="n">
-        <v>22062030.43464286</v>
+        <v>-8785.004537575207</v>
       </c>
       <c r="J45" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K45" t="inlineStr"/>
+        <v>14661470.04651263</v>
+      </c>
+      <c r="K45" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
         <v>2075</v>
       </c>
       <c r="B46" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C46" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D46" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E46" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F46" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G46" t="n">
-        <v>22589969.98813873</v>
+        <v>753366.7160678834</v>
       </c>
       <c r="H46" t="n">
-        <v>8916.779605832737</v>
+        <v>15574205.16926205</v>
       </c>
       <c r="I46" t="n">
-        <v>22396004.13071809</v>
+        <v>-8916.779605832737</v>
       </c>
       <c r="J46" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K46" t="inlineStr"/>
+        <v>14902632.43723741</v>
+      </c>
+      <c r="K46" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
         <v>2076</v>
       </c>
       <c r="B47" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C47" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D47" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E47" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F47" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G47" t="n">
-        <v>22928819.53796081</v>
+        <v>764667.2168089019</v>
       </c>
       <c r="H47" t="n">
-        <v>9050.531300501918</v>
+        <v>15807818.24680099</v>
       </c>
       <c r="I47" t="n">
-        <v>22734987.43223484</v>
+        <v>-9050.531300501918</v>
       </c>
       <c r="J47" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K47" t="inlineStr"/>
+        <v>15147412.2638227</v>
+      </c>
+      <c r="K47" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
         <v>2077</v>
       </c>
       <c r="B48" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C48" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D48" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E48" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F48" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G48" t="n">
-        <v>23272751.83103023</v>
+        <v>776137.2250610351</v>
       </c>
       <c r="H48" t="n">
-        <v>9186.289269528917</v>
+        <v>16044935.520503</v>
       </c>
       <c r="I48" t="n">
-        <v>23079055.48327328</v>
+        <v>-9186.289269528917</v>
       </c>
       <c r="J48" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K48" t="inlineStr"/>
+        <v>15395863.78780781</v>
+      </c>
+      <c r="K48" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
         <v>2078</v>
       </c>
       <c r="B49" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C49" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D49" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E49" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F49" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G49" t="n">
-        <v>23621843.10849567</v>
+        <v>787779.283436951</v>
       </c>
       <c r="H49" t="n">
-        <v>9324.083609355879</v>
+        <v>16285609.55331055</v>
       </c>
       <c r="I49" t="n">
-        <v>23428284.55507855</v>
+        <v>-9324.083609355879</v>
       </c>
       <c r="J49" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K49" t="inlineStr"/>
+        <v>15648042.08465145</v>
+      </c>
+      <c r="K49" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
         <v>2079</v>
       </c>
       <c r="B50" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C50" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D50" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E50" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F50" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G50" t="n">
-        <v>23976170.75512311</v>
+        <v>799595.9726885048</v>
       </c>
       <c r="H50" t="n">
-        <v>9463.944863234872</v>
+        <v>16529893.69661022</v>
       </c>
       <c r="I50" t="n">
-        <v>23782752.06295987</v>
+        <v>-9463.944863234872</v>
       </c>
       <c r="J50" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K50" t="inlineStr"/>
+        <v>15904003.05594879</v>
+      </c>
+      <c r="K50" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
         <v>2080</v>
       </c>
       <c r="B51" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C51" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D51" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E51" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F51" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G51" t="n">
-        <v>24335813.31644994</v>
+        <v>811589.9122788329</v>
       </c>
       <c r="H51" t="n">
-        <v>9605.904036402586</v>
+        <v>16777842.10205936</v>
       </c>
       <c r="I51" t="n">
-        <v>24142536.58345987</v>
+        <v>-9605.904036402586</v>
       </c>
       <c r="J51" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K51" t="inlineStr"/>
+        <v>16163803.4418151</v>
+      </c>
+      <c r="K51" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
         <v>2081</v>
       </c>
       <c r="B52" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C52" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D52" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E52" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F52" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G52" t="n">
-        <v>24700850.5161967</v>
+        <v>823763.7609630149</v>
       </c>
       <c r="H52" t="n">
-        <v>9749.992596080294</v>
+        <v>17029509.73359024</v>
       </c>
       <c r="I52" t="n">
-        <v>24507717.8717663</v>
+        <v>-9749.992596080294</v>
       </c>
       <c r="J52" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K52" t="inlineStr"/>
+        <v>16427500.83347048</v>
+      </c>
+      <c r="K52" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="n">
         <v>2082</v>
       </c>
       <c r="B53" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C53" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D53" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E53" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F53" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G53" t="n">
-        <v>25071363.27393963</v>
+        <v>836120.2173774597</v>
       </c>
       <c r="H53" t="n">
-        <v>9896.242484962489</v>
+        <v>17284952.37959408</v>
       </c>
       <c r="I53" t="n">
-        <v>24878376.87939812</v>
+        <v>-9896.242484962489</v>
       </c>
       <c r="J53" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K53" t="inlineStr"/>
+        <v>16695153.68599988</v>
+      </c>
+      <c r="K53" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="n">
         <v>2083</v>
       </c>
       <c r="B54" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C54" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D54" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E54" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F54" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G54" t="n">
-        <v>25447433.72304873</v>
+        <v>848662.0206381215</v>
       </c>
       <c r="H54" t="n">
-        <v>10044.68612290293</v>
+        <v>17544226.66528801</v>
       </c>
       <c r="I54" t="n">
-        <v>25254595.77214516</v>
+        <v>-10044.68612290293</v>
       </c>
       <c r="J54" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K54" t="inlineStr"/>
+        <v>16966821.33131653</v>
+      </c>
+      <c r="K54" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
         <v>2084</v>
       </c>
       <c r="B55" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C55" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D55" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E55" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F55" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G55" t="n">
-        <v>25829145.22889446</v>
+        <v>861391.9509476932</v>
       </c>
       <c r="H55" t="n">
-        <v>10195.35641365895</v>
+        <v>17807390.06526732</v>
       </c>
       <c r="I55" t="n">
-        <v>25636457.94828165</v>
+        <v>-10195.35641365895</v>
       </c>
       <c r="J55" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K55" t="inlineStr"/>
+        <v>17242563.99131466</v>
+      </c>
+      <c r="K55" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
         <v>2085</v>
       </c>
       <c r="B56" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C56" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D56" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E56" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F56" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G56" t="n">
-        <v>26216582.40732788</v>
+        <v>874312.8302119087</v>
       </c>
       <c r="H56" t="n">
-        <v>10348.28676006616</v>
+        <v>18074500.91624634</v>
       </c>
       <c r="I56" t="n">
-        <v>26024048.05706147</v>
+        <v>-10348.28676006616</v>
       </c>
       <c r="J56" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K56" t="inlineStr"/>
+        <v>17522442.79121149</v>
+      </c>
+      <c r="K56" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="n">
         <v>2086</v>
       </c>
       <c r="B57" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C57" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D57" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E57" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F57" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G57" t="n">
-        <v>26609831.14343779</v>
+        <v>887427.5226650873</v>
       </c>
       <c r="H57" t="n">
-        <v>10503.51106235235</v>
+        <v>18345618.42999003</v>
       </c>
       <c r="I57" t="n">
-        <v>26417452.01747367</v>
+        <v>-10503.51106235235</v>
       </c>
       <c r="J57" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K57" t="inlineStr"/>
+        <v>17806519.77310607</v>
+      </c>
+      <c r="K57" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="n">
         <v>2087</v>
       </c>
       <c r="B58" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C58" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D58" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E58" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F58" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G58" t="n">
-        <v>27008978.61058936</v>
+        <v>900738.9355050636</v>
       </c>
       <c r="H58" t="n">
-        <v>10661.06372825391</v>
+        <v>18620802.70643988</v>
       </c>
       <c r="I58" t="n">
-        <v>26816757.03729114</v>
+        <v>-10661.06372825391</v>
       </c>
       <c r="J58" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K58" t="inlineStr"/>
+        <v>18094857.90972999</v>
+      </c>
+      <c r="K58" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="n">
         <v>2088</v>
       </c>
       <c r="B59" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C59" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D59" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E59" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F59" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G59" t="n">
-        <v>27414113.28974818</v>
+        <v>914250.0195376392</v>
       </c>
       <c r="H59" t="n">
-        <v>10820.97968313235</v>
+        <v>18900114.74703647</v>
       </c>
       <c r="I59" t="n">
-        <v>27222051.63240484</v>
+        <v>-10820.97968313235</v>
       </c>
       <c r="J59" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K59" t="inlineStr"/>
+        <v>18387521.11840428</v>
+      </c>
+      <c r="K59" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
         <v>2089</v>
       </c>
       <c r="B60" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C60" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D60" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E60" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F60" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G60" t="n">
-        <v>27825324.98909442</v>
+        <v>927963.769830704</v>
       </c>
       <c r="H60" t="n">
-        <v>10983.29437840462</v>
+        <v>19183616.46824202</v>
       </c>
       <c r="I60" t="n">
-        <v>27633425.64644635</v>
+        <v>-10983.29437840462</v>
       </c>
       <c r="J60" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K60" t="inlineStr"/>
+        <v>18684574.27520762</v>
+      </c>
+      <c r="K60" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
         <v>2090</v>
       </c>
       <c r="B61" t="n">
-        <v>-42449.29232872641</v>
+        <v>-26710.70556174604</v>
       </c>
       <c r="C61" t="n">
-        <v>9517.41690617211</v>
+        <v>5988.719875952155</v>
       </c>
       <c r="D61" t="n">
-        <v>-758480.7516095076</v>
+        <v>-796404.7891899834</v>
       </c>
       <c r="E61" t="n">
-        <v>593586.5283496506</v>
+        <v>-593586.5283496506</v>
       </c>
       <c r="F61" t="n">
-        <v>5056.538344063384</v>
+        <v>-5309.365261266556</v>
       </c>
       <c r="G61" t="n">
-        <v>28242704.86393083</v>
+        <v>941883.2263781644</v>
       </c>
       <c r="H61" t="n">
-        <v>11148.0437949153</v>
+        <v>19471370.71526565</v>
       </c>
       <c r="I61" t="n">
-        <v>28050970.27069927</v>
+        <v>-11148.0437949153</v>
       </c>
       <c r="J61" t="n">
-        <v>15893</v>
-      </c>
-      <c r="K61" t="inlineStr"/>
+        <v>18986083.2293622</v>
+      </c>
+      <c r="K61" t="n">
+        <v>15893</v>
+      </c>
+      <c r="L61" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2531,25 +2716,25 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-145540147.5</v>
+        <v>145943436.4992725</v>
       </c>
       <c r="B2" t="n">
-        <v>415607627.7222123</v>
+        <v>251064761.0038516</v>
       </c>
       <c r="C2" t="n">
-        <v>270067480.2222123</v>
+        <v>105121324.5045791</v>
       </c>
       <c r="D2" t="n">
-        <v>2.855621866964319</v>
+        <v>1.720288126866898</v>
       </c>
       <c r="E2" t="n">
-        <v>0.08652866431420692</v>
+        <v>0.05808558341221404</v>
       </c>
       <c r="F2" t="n">
-        <v>0.06567345974445525</v>
+        <v>0.03696552561348638</v>
       </c>
       <c r="G2" t="n">
-        <v>2044</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>